<commit_message>
Revised C code with dmeasure and rmeasure
In particular I use the bivariate normal measurement error code to add
this to the C code. The R code should reflect this.
</commit_message>
<xml_diff>
--- a/lbv_data.xlsx
+++ b/lbv_data.xlsx
@@ -21,19 +21,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>SUSJ</t>
+    <t>cumulative_time</t>
   </si>
   <si>
-    <t>RECJ</t>
+    <t>DSUSJ</t>
   </si>
   <si>
-    <t>SUSA</t>
+    <t>DRECJ</t>
   </si>
   <si>
-    <t>RECA</t>
+    <t>DSUSA</t>
   </si>
   <si>
-    <t>cumulative_time</t>
+    <t>DRECA</t>
   </si>
 </sst>
 </file>
@@ -408,9 +408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
@@ -421,21 +419,21 @@
     <col min="6" max="16384" width="20.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>